<commit_message>
Actualiza entidades.xlsx y añade esquema API.drawio
</commit_message>
<xml_diff>
--- a/Documentacion/entidades.xlsx
+++ b/Documentacion/entidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalo\Desktop\SOFT BOT BMS\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B145BB5F-CD3F-453B-9A14-1AF06A651E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10AAC4E-C904-48EE-A8E5-03F24207D168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64605" yWindow="8295" windowWidth="19320" windowHeight="13455" xr2:uid="{D0F350FA-0AAC-4151-8162-A5D1164657A4}"/>
+    <workbookView xWindow="5297" yWindow="2717" windowWidth="19320" windowHeight="13457" xr2:uid="{D0F350FA-0AAC-4151-8162-A5D1164657A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>object</t>
+  </si>
+  <si>
+    <t>presentValue</t>
   </si>
 </sst>
 </file>
@@ -483,12 +486,13 @@
   <dimension ref="E5:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="4" max="4" width="13.3828125" customWidth="1"/>
+    <col min="10" max="10" width="12.23046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="5:10" x14ac:dyDescent="0.4">
@@ -552,6 +556,9 @@
       <c r="E11" t="s">
         <v>12</v>
       </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="5:10" x14ac:dyDescent="0.4">
       <c r="E15" s="1" t="s">
@@ -612,6 +619,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001A8ACF876485AF4BACC866FF4BC12D95" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="18943dcee2c8440bd100daa77ae38357">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1d675ff8-f6c9-4bac-af7b-be09e238b4c8" xmlns:ns4="572a4d6c-0f5d-46ee-8476-bf07411766ba" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df13328b1166cbf7632000dbd01b8097" ns3:_="" ns4:_="">
     <xsd:import namespace="1d675ff8-f6c9-4bac-af7b-be09e238b4c8"/>
@@ -844,15 +860,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -862,6 +869,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7820ABA4-4D4E-4C14-BB9F-B3B05797DB24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AEF8F30-477A-42F8-B043-8AD52CADB833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -880,14 +895,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7820ABA4-4D4E-4C14-BB9F-B3B05797DB24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E6A322-09DF-4A37-BB1C-7352D4181405}">
   <ds:schemaRefs>

</xml_diff>